<commit_message>
V9 - Updated Code with Wende Brief document.
</commit_message>
<xml_diff>
--- a/Data/2024.xlsx
+++ b/Data/2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ewong-c\Documents\UiPath\3DCA_Workflow\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4438BF47-5DEB-4536-A118-879D6B4441E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C998D95B-02AD-4445-B9B4-FDFE292FEB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2310" yWindow="1770" windowWidth="13500" windowHeight="8430" xr2:uid="{E8CBB2DA-08CF-44E8-942C-C162F7C1F40C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E8CBB2DA-08CF-44E8-942C-C162F7C1F40C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -460,6 +460,10 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="37.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>